<commit_message>
Toevoeging lijst To Do
</commit_message>
<xml_diff>
--- a/To Do/Steven Verheyen.xlsx
+++ b/To Do/Steven Verheyen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>Prioriteit:</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>Template webbapplicatie maken</t>
+  </si>
+  <si>
+    <t>2 uur</t>
+  </si>
+  <si>
+    <t>4,5 uur</t>
+  </si>
+  <si>
+    <t>Werken aan template webapplicatie</t>
+  </si>
+  <si>
+    <t>Anke A, Robbie V, Steven V</t>
   </si>
 </sst>
 </file>
@@ -320,51 +332,25 @@
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="17">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -447,226 +433,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -872,13 +638,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -965,14 +731,14 @@
     <sortCondition ref="D1:D38"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Opmerking" dataDxfId="30"/>
+    <tableColumn id="1" name="Opmerking" dataDxfId="2"/>
     <tableColumn id="2" name="Geschatte tijd"/>
     <tableColumn id="5" name="Werkelijke tijd"/>
     <tableColumn id="9" name="Voltooid"/>
     <tableColumn id="6" name="Prioriteit"/>
-    <tableColumn id="3" name="Deelnemers" dataDxfId="29"/>
+    <tableColumn id="3" name="Deelnemers" dataDxfId="1"/>
     <tableColumn id="4" name="Solved"/>
-    <tableColumn id="8" name="APP" dataDxfId="28"/>
+    <tableColumn id="8" name="APP" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1268,7 +1034,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1044,7 @@
     <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -1497,11 +1263,11 @@
       </c>
       <c r="I7" s="12">
         <f>COUNTIFS(G2:G38,"In Process")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="13">
         <f>I7/$I$10</f>
-        <v>0.14285714285714285</v>
+        <v>0</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>11</v>
@@ -1530,18 +1296,18 @@
         <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="10">
         <f>COUNTIFS(G2:G38,"Fixed")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="8">
         <f>I8/$I$10</f>
-        <v>0.14285714285714285</v>
+        <v>0.25</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>5</v>
@@ -1554,19 +1320,37 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="E9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="23">
+        <v>41361</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I9" s="17">
         <f>COUNTIFS(A2:G2038,"Solved")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J9" s="18">
         <f>I9/$I$10</f>
-        <v>0.7142857142857143</v>
+        <v>0.75</v>
       </c>
       <c r="K9" s="19" t="s">
         <v>3</v>
@@ -1587,7 +1371,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="20">
         <f>SUM(I6:I9)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J10" s="21">
         <v>1</v>
@@ -1849,52 +1633,52 @@
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="G9:G41 G1:G7">
-    <cfRule type="cellIs" dxfId="37" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="36" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="37" operator="equal">
       <formula>"In Process"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="38" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:H7 A9:H1048576">
-    <cfRule type="expression" dxfId="34" priority="29">
+    <cfRule type="expression" dxfId="13" priority="29">
       <formula>$G1="Solved"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="30">
+    <cfRule type="expression" dxfId="12" priority="30">
       <formula>$G1="Not Started"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="31">
+    <cfRule type="expression" dxfId="11" priority="31">
       <formula>$G1="In Process"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="10" priority="32">
       <formula>$G1="Fixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"In Process"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:H8">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$G8="Solved"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$G8="Not Started"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$G8="In Process"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$G8="Fixed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Aanvulling lijst To Do
</commit_message>
<xml_diff>
--- a/To Do/Steven Verheyen.xlsx
+++ b/To Do/Steven Verheyen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>Prioriteit:</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Werken website eigen gedeelte</t>
+  </si>
+  <si>
+    <t>Nazicht mock-ups</t>
+  </si>
+  <si>
+    <t>30 minuten</t>
   </si>
 </sst>
 </file>
@@ -653,7 +659,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1043,7 +1049,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,7 +1322,7 @@
       </c>
       <c r="J8" s="8">
         <f>I8/$I$10</f>
-        <v>0.2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>5</v>
@@ -1355,11 +1361,11 @@
       </c>
       <c r="I9" s="17">
         <f>COUNTIFS(A2:G2038,"Solved")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J9" s="18">
         <f>I9/$I$10</f>
-        <v>0.8</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="K9" s="19" t="s">
         <v>3</v>
@@ -1398,7 +1404,7 @@
       </c>
       <c r="I10" s="20">
         <f>SUM(I6:I9)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J10" s="21">
         <v>1</v>
@@ -1434,20 +1440,56 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="23">
+        <v>41363</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="E13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="23">
+        <v>41364</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>

</xml_diff>